<commit_message>
improved management of presidential mandates
</commit_message>
<xml_diff>
--- a/in/extraction1/corrections/supp_PRF.xlsx
+++ b/in/extraction1/corrections/supp_PRF.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="59">
   <si>
     <t>Code sexe</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>EUR_0000916</t>
+  </si>
+  <si>
+    <t>Date deces</t>
   </si>
 </sst>
 </file>
@@ -1032,11 +1035,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,22 +1047,23 @@
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1069,47 +1073,50 @@
       <c r="C1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1119,33 +1126,33 @@
       <c r="C2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11">
+        <v>25881</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="9">
+      <c r="I2" s="9">
         <v>21540</v>
       </c>
-      <c r="I2" s="11">
+      <c r="J2" s="11">
         <v>24094</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1155,11 +1162,14 @@
       <c r="O2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1169,33 +1179,33 @@
       <c r="C3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11">
+        <v>25881</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
       <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>24095</v>
       </c>
-      <c r="I3" s="11">
+      <c r="J3" s="11">
         <v>25321</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1205,11 +1215,14 @@
       <c r="O3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1219,33 +1232,33 @@
       <c r="C4" s="11">
         <v>3395</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="11">
+        <v>35408</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
       <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>25322</v>
       </c>
-      <c r="I4" s="11">
+      <c r="J4" s="11">
         <v>25368</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1255,11 +1268,14 @@
       <c r="O4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1269,33 +1285,33 @@
       <c r="C5" s="11">
         <v>4204</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11">
+        <v>27121</v>
+      </c>
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>25369</v>
       </c>
-      <c r="I5" s="11">
+      <c r="J5" s="11">
         <v>27121</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>43</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1305,11 +1321,14 @@
       <c r="O5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1319,33 +1338,33 @@
       <c r="C6" s="11">
         <v>3395</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="11">
+        <v>35408</v>
+      </c>
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>27122</v>
       </c>
-      <c r="I6" s="11">
+      <c r="J6" s="11">
         <v>27167</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>32</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1355,11 +1374,14 @@
       <c r="O6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1369,47 +1391,50 @@
       <c r="C7" s="11">
         <v>9530</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
       <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>27168</v>
       </c>
-      <c r="I7" s="11">
+      <c r="J7" s="11">
         <v>29715</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>27</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="5">
+      <c r="M7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="5">
         <v>1030</v>
       </c>
-      <c r="N7" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="O7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1419,33 +1444,33 @@
       <c r="C8" s="11">
         <v>6144</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="11">
+        <v>35072</v>
+      </c>
+      <c r="E8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>29716</v>
       </c>
-      <c r="I8" s="11">
+      <c r="J8" s="11">
         <v>32270</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>27</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1455,11 +1480,14 @@
       <c r="O8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1469,33 +1497,33 @@
       <c r="C9" s="11">
         <v>6144</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="11">
+        <v>35072</v>
+      </c>
+      <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
       <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>32271</v>
       </c>
-      <c r="I9" s="11">
+      <c r="J9" s="11">
         <v>34825</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1505,11 +1533,14 @@
       <c r="O9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1519,47 +1550,50 @@
       <c r="C10" s="11">
         <v>12022</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="11">
+        <v>43734</v>
+      </c>
+      <c r="E10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
       <c r="F10" t="s">
         <v>11</v>
       </c>
       <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>34826</v>
       </c>
-      <c r="I10" s="11">
+      <c r="J10" s="11">
         <v>37380</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>27</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="5">
+      <c r="M10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="5">
         <v>916</v>
       </c>
-      <c r="N10" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="O10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1569,47 +1603,50 @@
       <c r="C11" s="11">
         <v>12022</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="11">
+        <v>43734</v>
+      </c>
+      <c r="E11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>37381</v>
       </c>
-      <c r="I11" s="11">
+      <c r="J11" s="11">
         <v>39207</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>27</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="5">
+      <c r="M11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="5">
         <v>916</v>
       </c>
-      <c r="N11" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="O11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1619,47 +1656,50 @@
       <c r="C12" s="11">
         <v>20117</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>39208</v>
       </c>
-      <c r="I12" s="11">
+      <c r="J12" s="11">
         <v>41034</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>27</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="5">
+      <c r="M12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="5">
         <v>4339</v>
       </c>
-      <c r="N12" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="O12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1669,47 +1709,50 @@
       <c r="C13" s="11">
         <v>19948</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
       <c r="F13" t="s">
         <v>11</v>
       </c>
       <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>41035</v>
       </c>
-      <c r="I13" s="11">
+      <c r="J13" s="11">
         <v>42861</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>27</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="5">
+      <c r="M13" s="5">
         <v>724</v>
       </c>
-      <c r="M13" s="5">
+      <c r="N13" s="5">
         <v>4285</v>
       </c>
-      <c r="N13" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="O13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1719,33 +1762,33 @@
       <c r="C14" s="11">
         <v>28480</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
       <c r="F14" t="s">
         <v>11</v>
       </c>
       <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>42862</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="J14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" t="s">
         <v>27</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="M14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1755,7 +1798,10 @@
       <c r="O14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>